<commit_message>
Add market building for ships and relinking
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-ships.xlsx
+++ b/premise/data/additional_inventories/lci-ships.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{807AC885-4185-9949-A8A3-25A50053BE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F7C9D57-C6D1-7C45-82AB-6B1F4B59595C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34260" yWindow="-920" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1019,8 +1019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O273"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A170" workbookViewId="0">
-      <selection activeCell="B182" sqref="B182"/>
+    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
+      <selection activeCell="B150" sqref="B150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fix uncertainty in inventories
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-ships.xlsx
+++ b/premise/data/additional_inventories/lci-ships.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10526"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA81D883-22D7-C34C-BD65-0B4FBBF90690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{269EC39B-B4CF-0948-B675-5D6B79FB850C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35060" yWindow="-480" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="inventories" sheetId="1" r:id="rId1"/>
@@ -1034,8 +1034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O273"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A210" workbookViewId="0">
-      <selection activeCell="D232" sqref="D232"/>
+    <sheetView tabSelected="1" topLeftCell="A241" workbookViewId="0">
+      <selection activeCell="L274" sqref="L274"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2215,12 +2215,12 @@
         <v>3.472222222222222E-8</v>
       </c>
       <c r="K77" s="9">
-        <f>350000/B65</f>
-        <v>2.2875816993464053E-6</v>
+        <f>3500/B65</f>
+        <v>2.2875816993464053E-8</v>
       </c>
       <c r="L77" s="9">
-        <f>1000000/B64</f>
-        <v>7.4074074074074075E-6</v>
+        <f>10000/B64</f>
+        <v>7.4074074074074073E-8</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.2">
@@ -4723,12 +4723,12 @@
         <v>1.0925271739130437E-5</v>
       </c>
       <c r="K206" s="6">
-        <f>0.00186*(B201*43*B196/3.6)</f>
-        <v>2.0321005434782613E-5</v>
+        <f>0.0009*(B201*43*B196/3.6)</f>
+        <v>9.8327445652173915E-6</v>
       </c>
       <c r="L206" s="6">
-        <f>0.00186*(B201*43*B197/3.6)</f>
-        <v>2.4836784420289866E-5</v>
+        <f>0.0009*(B201*43*B197/3.6)</f>
+        <v>1.2017798913043482E-5</v>
       </c>
     </row>
     <row r="207" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -4759,12 +4759,12 @@
         <v>3.1561896135265709E-5</v>
       </c>
       <c r="K207" s="6">
-        <f>0.00186*(B201*43*B196/3.6)</f>
-        <v>2.0321005434782613E-5</v>
+        <f>0.0026*(B201*43*B196/3.6)</f>
+        <v>2.8405706521739134E-5</v>
       </c>
       <c r="L207" s="6">
-        <f>0.00186*(B201*43*B197/3.6)</f>
-        <v>2.4836784420289866E-5</v>
+        <f>0.0026*(B201*43*B197/3.6)</f>
+        <v>3.4718085748792285E-5</v>
       </c>
     </row>
     <row r="208" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -4795,12 +4795,12 @@
         <v>3.0347977053140105E-6</v>
       </c>
       <c r="K208" s="6">
-        <f>0.00186*(B201*43*B196/3.6)</f>
-        <v>2.0321005434782613E-5</v>
+        <f>0.00025*(B201*43*B196/3.6)</f>
+        <v>2.7313179347826089E-6</v>
       </c>
       <c r="L208" s="6">
-        <f>0.00186*(B201*43*B197/3.6)</f>
-        <v>2.4836784420289866E-5</v>
+        <f>0.00025*(B201*43*B197/3.6)</f>
+        <v>3.3382774758454117E-6</v>
       </c>
     </row>
     <row r="209" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -4831,12 +4831,12 @@
         <v>1.2139190821256042E-7</v>
       </c>
       <c r="K209" s="6">
-        <f>0.00186*(B201*43*B196/3.6)</f>
-        <v>2.0321005434782613E-5</v>
+        <f>0.00001*(B201*43*B196/3.6)</f>
+        <v>1.0925271739130436E-7</v>
       </c>
       <c r="L209" s="6">
-        <f>0.00186*(B201*43*B197/3.6)</f>
-        <v>2.4836784420289866E-5</v>
+        <f>0.00001*(B201*43*B197/3.6)</f>
+        <v>1.3353109903381649E-7</v>
       </c>
     </row>
     <row r="210" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -4867,12 +4867,12 @@
         <v>4.9770682367149768E-6</v>
       </c>
       <c r="K210" s="6">
-        <f>0.00186*(B201*43*B196/3.6)</f>
-        <v>2.0321005434782613E-5</v>
+        <f>0.0004*(B201*43*B196/3.6)</f>
+        <v>4.3701086956521745E-6</v>
       </c>
       <c r="L210" s="6">
-        <f>0.00186*(B201*43*B197/3.6)</f>
-        <v>2.4836784420289866E-5</v>
+        <f>0.0004*(B201*43*B197/3.6)</f>
+        <v>5.3412439613526591E-6</v>
       </c>
     </row>
     <row r="211" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -4903,12 +4903,12 @@
         <v>3.6417572463768126E-7</v>
       </c>
       <c r="K211" s="6">
-        <f>0.00186*(B201*43*B196/3.6)</f>
-        <v>2.0321005434782613E-5</v>
+        <f>0.00003*(B201*43*B196/3.6)</f>
+        <v>3.2775815217391311E-7</v>
       </c>
       <c r="L211" s="6">
-        <f>0.00186*(B201*43*B197/3.6)</f>
-        <v>2.4836784420289866E-5</v>
+        <f>0.00003*(B201*43*B197/3.6)</f>
+        <v>4.0059329710144941E-7</v>
       </c>
     </row>
     <row r="213" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -5296,12 +5296,12 @@
         <v>1.0925271739130437E-5</v>
       </c>
       <c r="K237" s="6">
-        <f>0.00186*(B232*43*B227/3.6)</f>
-        <v>2.0321005434782613E-5</v>
+        <f>0.0009*(B232*43*B227/3.6)</f>
+        <v>9.8327445652173915E-6</v>
       </c>
       <c r="L237" s="6">
-        <f>0.00186*(B232*43*B228/3.6)</f>
-        <v>2.4836784420289866E-5</v>
+        <f>0.0009*(B232*43*B228/3.6)</f>
+        <v>1.2017798913043482E-5</v>
       </c>
     </row>
     <row r="238" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -5332,12 +5332,12 @@
         <v>3.1561896135265709E-5</v>
       </c>
       <c r="K238" s="6">
-        <f>0.00186*(B232*43*B227/3.6)</f>
-        <v>2.0321005434782613E-5</v>
+        <f>0.0026*(B232*43*B227/3.6)</f>
+        <v>2.8405706521739134E-5</v>
       </c>
       <c r="L238" s="6">
-        <f>0.00186*(B232*43*B228/3.6)</f>
-        <v>2.4836784420289866E-5</v>
+        <f>0.0026*(B232*43*B228/3.6)</f>
+        <v>3.4718085748792285E-5</v>
       </c>
     </row>
     <row r="239" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -5368,12 +5368,12 @@
         <v>3.0347977053140105E-6</v>
       </c>
       <c r="K239" s="6">
-        <f>0.00186*(B232*43*B227/3.6)</f>
-        <v>2.0321005434782613E-5</v>
+        <f>0.00025*(B232*43*B227/3.6)</f>
+        <v>2.7313179347826089E-6</v>
       </c>
       <c r="L239" s="6">
-        <f>0.00186*(B232*43*B228/3.6)</f>
-        <v>2.4836784420289866E-5</v>
+        <f>0.00025*(B232*43*B228/3.6)</f>
+        <v>3.3382774758454117E-6</v>
       </c>
     </row>
     <row r="240" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -5404,12 +5404,12 @@
         <v>1.2139190821256042E-7</v>
       </c>
       <c r="K240" s="6">
-        <f>0.00186*(B232*43*B227/3.6)</f>
-        <v>2.0321005434782613E-5</v>
+        <f>0.00001*(B232*43*B227/3.6)</f>
+        <v>1.0925271739130436E-7</v>
       </c>
       <c r="L240" s="6">
-        <f>0.00186*(B232*43*B228/3.6)</f>
-        <v>2.4836784420289866E-5</v>
+        <f>0.00001*(B232*43*B228/3.6)</f>
+        <v>1.3353109903381649E-7</v>
       </c>
     </row>
     <row r="241" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -5440,12 +5440,12 @@
         <v>4.9770682367149768E-6</v>
       </c>
       <c r="K241" s="6">
-        <f>0.00186*(B232*43*B227/3.6)</f>
-        <v>2.0321005434782613E-5</v>
+        <f>0.00041*(B232*43*B227/3.6)</f>
+        <v>4.4793614130434786E-6</v>
       </c>
       <c r="L241" s="6">
-        <f>0.00186*(B232*43*B228/3.6)</f>
-        <v>2.4836784420289866E-5</v>
+        <f>0.00041*(B232*43*B228/3.6)</f>
+        <v>5.4747750603864751E-6</v>
       </c>
     </row>
     <row r="242" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -5476,12 +5476,12 @@
         <v>3.6417572463768126E-7</v>
       </c>
       <c r="K242" s="6">
-        <f>0.00186*(B232*43*B227/3.6)</f>
-        <v>2.0321005434782613E-5</v>
+        <f>0.00003*(B232*43*B227/3.6)</f>
+        <v>3.2775815217391311E-7</v>
       </c>
       <c r="L242" s="6">
-        <f>0.00186*(B232*43*B228/3.6)</f>
-        <v>2.4836784420289866E-5</v>
+        <f>0.00003*(B232*43*B228/3.6)</f>
+        <v>4.0059329710144941E-7</v>
       </c>
     </row>
     <row r="244" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -5869,12 +5869,12 @@
         <v>1.0925271739130437E-5</v>
       </c>
       <c r="K268" s="6">
-        <f>0.00186*(B263*43*B258/3.6)</f>
-        <v>2.0321005434782613E-5</v>
+        <f>0.0009*(B263*43*B258/3.6)</f>
+        <v>9.8327445652173915E-6</v>
       </c>
       <c r="L268" s="6">
-        <f>0.00186*(B263*43*B259/3.6)</f>
-        <v>2.4836784420289866E-5</v>
+        <f>0.0009*(B263*43*B259/3.6)</f>
+        <v>1.2017798913043482E-5</v>
       </c>
     </row>
     <row r="269" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -5905,12 +5905,12 @@
         <v>3.1561896135265709E-5</v>
       </c>
       <c r="K269" s="6">
-        <f>0.00186*(B263*43*B258/3.6)</f>
-        <v>2.0321005434782613E-5</v>
+        <f>0.0026*(B263*43*B258/3.6)</f>
+        <v>2.8405706521739134E-5</v>
       </c>
       <c r="L269" s="6">
-        <f>0.00186*(B263*43*B259/3.6)</f>
-        <v>2.4836784420289866E-5</v>
+        <f>0.0026*(B263*43*B259/3.6)</f>
+        <v>3.4718085748792285E-5</v>
       </c>
     </row>
     <row r="270" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -5941,12 +5941,12 @@
         <v>3.0347977053140105E-6</v>
       </c>
       <c r="K270" s="6">
-        <f>0.00186*(B263*43*B258/3.6)</f>
-        <v>2.0321005434782613E-5</v>
+        <f>0.00025*(B263*43*B258/3.6)</f>
+        <v>2.7313179347826089E-6</v>
       </c>
       <c r="L270" s="6">
-        <f>0.00186*(B263*43*B259/3.6)</f>
-        <v>2.4836784420289866E-5</v>
+        <f>0.00025*(B263*43*B259/3.6)</f>
+        <v>3.3382774758454117E-6</v>
       </c>
     </row>
     <row r="271" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -5977,12 +5977,12 @@
         <v>1.2139190821256042E-7</v>
       </c>
       <c r="K271" s="6">
-        <f>0.00186*(B263*43*B258/3.6)</f>
-        <v>2.0321005434782613E-5</v>
+        <f>0.00001*(B263*43*B258/3.6)</f>
+        <v>1.0925271739130436E-7</v>
       </c>
       <c r="L271" s="6">
-        <f>0.00186*(B263*43*B259/3.6)</f>
-        <v>2.4836784420289866E-5</v>
+        <f>0.00001*(B263*43*B259/3.6)</f>
+        <v>1.3353109903381649E-7</v>
       </c>
     </row>
     <row r="272" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -6013,12 +6013,12 @@
         <v>4.9770682367149768E-6</v>
       </c>
       <c r="K272" s="6">
-        <f>0.00186*(B263*43*B258/3.6)</f>
-        <v>2.0321005434782613E-5</v>
+        <f>0.00041*(B263*43*B258/3.6)</f>
+        <v>4.4793614130434786E-6</v>
       </c>
       <c r="L272" s="6">
-        <f>0.00186*(B263*43*B259/3.6)</f>
-        <v>2.4836784420289866E-5</v>
+        <f>0.00041*(B263*43*B259/3.6)</f>
+        <v>5.4747750603864751E-6</v>
       </c>
     </row>
     <row r="273" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -6049,12 +6049,12 @@
         <v>3.6417572463768126E-7</v>
       </c>
       <c r="K273" s="6">
-        <f>0.00186*(B263*43*B258/3.6)</f>
-        <v>2.0321005434782613E-5</v>
+        <f>0.00003*(B263*43*B258/3.6)</f>
+        <v>3.2775815217391311E-7</v>
       </c>
       <c r="L273" s="6">
-        <f>0.00186*(B263*43*B259/3.6)</f>
-        <v>2.4836784420289866E-5</v>
+        <f>0.00003*(B263*43*B259/3.6)</f>
+        <v>4.0059329710144941E-7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>